<commit_message>
refactor: arbiter schema details
</commit_message>
<xml_diff>
--- a/OCABundles/schema/credebl/arbiter/Arbiter.xlsx
+++ b/OCABundles/schema/credebl/arbiter/Arbiter.xlsx
@@ -1168,7 +1168,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>Winner</t>
+    <t>Arbiter</t>
   </si>
   <si>
     <t>Full Name</t>
@@ -2190,7 +2190,7 @@
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="48" fillId="9" fontId="18" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="49" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -2205,7 +2205,7 @@
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="33" fillId="9" fontId="18" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="52" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>

</xml_diff>